<commit_message>
Cucumber reports will be stored in "CucumberReports" folder
</commit_message>
<xml_diff>
--- a/Myntra.xlsx
+++ b/Myntra.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="173">
   <si>
     <t>Shirts</t>
   </si>
@@ -518,6 +518,33 @@
   </si>
   <si>
     <t xml:space="preserve"> 15500</t>
+  </si>
+  <si>
+    <t>Cottinfab</t>
+  </si>
+  <si>
+    <t>Women White &amp; Blue Striped Lightweight Cotton Open Front Jacket</t>
+  </si>
+  <si>
+    <t>799</t>
+  </si>
+  <si>
+    <t>H&amp;M</t>
+  </si>
+  <si>
+    <t>Puffer Gilet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1499</t>
+  </si>
+  <si>
+    <t>The Indian Garage Co</t>
+  </si>
+  <si>
+    <t>Men Peach-Coloured &amp; White Comfort Fit Checked Casual Shirt</t>
+  </si>
+  <si>
+    <t>682</t>
   </si>
 </sst>
 </file>
@@ -616,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -641,6 +668,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyBorder="true" applyFill="true">
       <alignment wrapText="true" vertical="top" horizontal="left"/>
@@ -1010,7 +1064,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95572E08-B2A5-42D5-8863-DC8E08610FF4}">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
       <selection activeCell="C62" sqref="C62"/>
@@ -1731,6 +1785,39 @@
         <v>163</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="s" s="12">
+        <v>164</v>
+      </c>
+      <c r="B65" t="s" s="13">
+        <v>165</v>
+      </c>
+      <c r="C65" t="s" s="14">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="15">
+        <v>167</v>
+      </c>
+      <c r="B66" t="s" s="16">
+        <v>168</v>
+      </c>
+      <c r="C66" t="s" s="17">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="18">
+        <v>170</v>
+      </c>
+      <c r="B67" t="s" s="19">
+        <v>171</v>
+      </c>
+      <c r="C67" t="s" s="20">
+        <v>172</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>